<commit_message>
feat: adiciona nome no excel de saída
</commit_message>
<xml_diff>
--- a/api/automation/alleasy_model_excel/model.xlsx
+++ b/api/automation/alleasy_model_excel/model.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26611"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_162a\AC\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projetos_random\py-alleasy-hours-automation-v2\api\automation\alleasy_model_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A6E4DC09-D8D6-4458-A170-01A64EAB281C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" tabRatio="484" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" tabRatio="484"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,18 +32,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
   <si>
     <t>EMPRESA:</t>
   </si>
   <si>
-    <t>Viveo/ AzimuteMed</t>
-  </si>
-  <si>
     <t xml:space="preserve">REPRESENTANTE: </t>
-  </si>
-  <si>
-    <t>Gabriel Campera da Silva</t>
   </si>
   <si>
     <t>Período:</t>
@@ -103,16 +96,19 @@
   <si>
     <t>TOTAL</t>
   </si>
+  <si>
+    <t>Viveo / Humania</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[hh]:mm"/>
     <numFmt numFmtId="165" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1021,9 +1017,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1061,9 +1057,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1098,7 +1094,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1133,7 +1129,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1306,57 +1302,55 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S49"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A29" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="P33" sqref="P33:P41"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" style="20" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" style="20" customWidth="1"/>
     <col min="2" max="2" width="12" style="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" style="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.42578125" style="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.44140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" style="20" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13" style="20" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" style="20" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" style="20" customWidth="1"/>
-    <col min="10" max="12" width="8.85546875" style="20" customWidth="1"/>
-    <col min="13" max="13" width="11.85546875" style="17" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" style="3" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.109375" style="20" customWidth="1"/>
+    <col min="10" max="12" width="8.88671875" style="20" customWidth="1"/>
+    <col min="13" max="13" width="11.88671875" style="17" customWidth="1"/>
+    <col min="14" max="14" width="10.6640625" style="3" hidden="1" customWidth="1"/>
     <col min="15" max="15" width="14" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="67.140625" customWidth="1"/>
+    <col min="16" max="16" width="67.109375" customWidth="1"/>
     <col min="21" max="21" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="35" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="26" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:19">
-      <c r="A2" s="26" t="s">
+      <c r="B2" s="35"/>
+    </row>
+    <row r="4" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="27" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" s="35" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" ht="15.75">
-      <c r="A4" s="27" t="s">
-        <v>4</v>
       </c>
       <c r="B4" s="31">
         <v>45078</v>
       </c>
       <c r="C4" s="57" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D4" s="58"/>
       <c r="E4" s="28">
@@ -1377,27 +1371,27 @@
       <c r="R4" s="2"/>
       <c r="S4" s="2"/>
     </row>
-    <row r="5" spans="1:19" ht="25.5">
+    <row r="5" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="59" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B5" s="60"/>
       <c r="C5" s="60"/>
       <c r="D5" s="61"/>
       <c r="E5" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="29" t="s">
+      <c r="H5" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="29" t="s">
+      <c r="I5" s="30" t="s">
         <v>9</v>
-      </c>
-      <c r="H5" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="I5" s="30" t="s">
-        <v>11</v>
       </c>
       <c r="J5" s="17"/>
       <c r="K5" s="18"/>
@@ -1410,7 +1404,7 @@
       <c r="R5" s="2"/>
       <c r="S5" s="2"/>
     </row>
-    <row r="6" spans="1:19" ht="15.75">
+    <row r="6" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="62"/>
       <c r="B6" s="63"/>
       <c r="C6" s="63"/>
@@ -1442,69 +1436,69 @@
       <c r="R6" s="2"/>
       <c r="S6" s="2"/>
     </row>
-    <row r="7" spans="1:19" ht="13.5" thickBot="1"/>
-    <row r="8" spans="1:19" ht="13.5" thickBot="1">
+    <row r="7" spans="1:19" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:19" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="22"/>
       <c r="B8" s="4"/>
       <c r="C8" s="80" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D8" s="81"/>
       <c r="E8" s="78" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F8" s="79"/>
       <c r="G8" s="79"/>
       <c r="H8" s="79"/>
       <c r="I8" s="80" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J8" s="81"/>
       <c r="K8" s="82" t="s">
+        <v>12</v>
+      </c>
+      <c r="L8" s="82" t="s">
+        <v>13</v>
+      </c>
+      <c r="M8" s="82" t="s">
         <v>14</v>
-      </c>
-      <c r="L8" s="82" t="s">
-        <v>15</v>
-      </c>
-      <c r="M8" s="82" t="s">
-        <v>16</v>
       </c>
       <c r="N8" s="7"/>
       <c r="O8" s="5"/>
       <c r="P8" s="65" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="11" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" ht="26.25" thickBot="1">
-      <c r="A9" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>19</v>
-      </c>
       <c r="C9" s="14" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J9" s="13" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="K9" s="83"/>
       <c r="L9" s="83"/>
@@ -1513,7 +1507,7 @@
       <c r="O9" s="6"/>
       <c r="P9" s="66"/>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="43"/>
       <c r="B10" s="37"/>
       <c r="C10" s="38"/>
@@ -1531,7 +1525,7 @@
       <c r="O10" s="45"/>
       <c r="P10" s="46"/>
     </row>
-    <row r="11" spans="1:19" ht="15.75">
+    <row r="11" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="47" t="str">
         <f>IF(WEEKDAY(B11)=1,"domingo",IF(WEEKDAY(B11)=2,"segunda-feira",IF(WEEKDAY(B11)=3,"terça-feira",IF(WEEKDAY(B11)=4,"quarta-feira",IF(WEEKDAY(B11)=5,"quinta-feira",IF(WEEKDAY(B11)=6,"sexta-feira",IF(WEEKDAY(B11)=7,"sábado","")))))))</f>
         <v>quinta-feira</v>
@@ -1555,7 +1549,7 @@
       <c r="O11" s="52"/>
       <c r="P11" s="53"/>
     </row>
-    <row r="12" spans="1:19" ht="15.75">
+    <row r="12" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="47" t="str">
         <f t="shared" ref="A12:A38" si="0">IF(WEEKDAY(B12)=1,"domingo",IF(WEEKDAY(B12)=2,"segunda-feira",IF(WEEKDAY(B12)=3,"terça-feira",IF(WEEKDAY(B12)=4,"quarta-feira",IF(WEEKDAY(B12)=5,"quinta-feira",IF(WEEKDAY(B12)=6,"sexta-feira",IF(WEEKDAY(B12)=7,"sábado","")))))))</f>
         <v>sexta-feira</v>
@@ -1579,7 +1573,7 @@
       <c r="O12" s="52"/>
       <c r="P12" s="53"/>
     </row>
-    <row r="13" spans="1:19" ht="15.75">
+    <row r="13" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="36" t="str">
         <f t="shared" si="0"/>
         <v>sábado</v>
@@ -1603,7 +1597,7 @@
       <c r="O13" s="41"/>
       <c r="P13" s="42"/>
     </row>
-    <row r="14" spans="1:19" ht="15.75">
+    <row r="14" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="36" t="str">
         <f t="shared" si="0"/>
         <v>domingo</v>
@@ -1627,7 +1621,7 @@
       <c r="O14" s="41"/>
       <c r="P14" s="42"/>
     </row>
-    <row r="15" spans="1:19" ht="15.75">
+    <row r="15" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="36" t="str">
         <f t="shared" si="0"/>
         <v>segunda-feira</v>
@@ -1651,7 +1645,7 @@
       <c r="O15" s="41"/>
       <c r="P15" s="42"/>
     </row>
-    <row r="16" spans="1:19" ht="15.75">
+    <row r="16" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="36" t="str">
         <f t="shared" si="0"/>
         <v>terça-feira</v>
@@ -1675,7 +1669,7 @@
       <c r="O16" s="41"/>
       <c r="P16" s="42"/>
     </row>
-    <row r="17" spans="1:16" ht="15.75">
+    <row r="17" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="36" t="str">
         <f t="shared" si="0"/>
         <v>quarta-feira</v>
@@ -1699,7 +1693,7 @@
       <c r="O17" s="41"/>
       <c r="P17" s="42"/>
     </row>
-    <row r="18" spans="1:16" ht="15.75">
+    <row r="18" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="47" t="str">
         <f t="shared" si="0"/>
         <v>quinta-feira</v>
@@ -1723,7 +1717,7 @@
       <c r="O18" s="52"/>
       <c r="P18" s="53"/>
     </row>
-    <row r="19" spans="1:16" ht="15.75">
+    <row r="19" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="47" t="str">
         <f t="shared" si="0"/>
         <v>sexta-feira</v>
@@ -1747,7 +1741,7 @@
       <c r="O19" s="52"/>
       <c r="P19" s="53"/>
     </row>
-    <row r="20" spans="1:16" ht="15.75">
+    <row r="20" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="36" t="str">
         <f t="shared" si="0"/>
         <v>sábado</v>
@@ -1771,7 +1765,7 @@
       <c r="O20" s="41"/>
       <c r="P20" s="42"/>
     </row>
-    <row r="21" spans="1:16" ht="15.75">
+    <row r="21" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="36" t="str">
         <f t="shared" si="0"/>
         <v>domingo</v>
@@ -1795,7 +1789,7 @@
       <c r="O21" s="41"/>
       <c r="P21" s="42"/>
     </row>
-    <row r="22" spans="1:16" ht="15.75">
+    <row r="22" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="36" t="str">
         <f t="shared" si="0"/>
         <v>segunda-feira</v>
@@ -1819,7 +1813,7 @@
       <c r="O22" s="41"/>
       <c r="P22" s="42"/>
     </row>
-    <row r="23" spans="1:16" ht="15.75">
+    <row r="23" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="36" t="str">
         <f t="shared" si="0"/>
         <v>terça-feira</v>
@@ -1843,7 +1837,7 @@
       <c r="O23" s="41"/>
       <c r="P23" s="42"/>
     </row>
-    <row r="24" spans="1:16" ht="15.75">
+    <row r="24" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="36" t="str">
         <f t="shared" si="0"/>
         <v>quarta-feira</v>
@@ -1867,7 +1861,7 @@
       <c r="O24" s="41"/>
       <c r="P24" s="42"/>
     </row>
-    <row r="25" spans="1:16" ht="15.75">
+    <row r="25" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="47" t="str">
         <f t="shared" si="0"/>
         <v>quinta-feira</v>
@@ -1891,7 +1885,7 @@
       <c r="O25" s="52"/>
       <c r="P25" s="53"/>
     </row>
-    <row r="26" spans="1:16" ht="15.75">
+    <row r="26" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="47" t="str">
         <f t="shared" si="0"/>
         <v>sexta-feira</v>
@@ -1915,7 +1909,7 @@
       <c r="O26" s="52"/>
       <c r="P26" s="53"/>
     </row>
-    <row r="27" spans="1:16" ht="15.75">
+    <row r="27" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="36" t="str">
         <f t="shared" si="0"/>
         <v>sábado</v>
@@ -1939,7 +1933,7 @@
       <c r="O27" s="41"/>
       <c r="P27" s="42"/>
     </row>
-    <row r="28" spans="1:16" ht="15.75">
+    <row r="28" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="36" t="str">
         <f t="shared" si="0"/>
         <v>domingo</v>
@@ -1963,7 +1957,7 @@
       <c r="O28" s="41"/>
       <c r="P28" s="42"/>
     </row>
-    <row r="29" spans="1:16" ht="15.75">
+    <row r="29" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="36" t="str">
         <f t="shared" si="0"/>
         <v>segunda-feira</v>
@@ -1987,7 +1981,7 @@
       <c r="O29" s="41"/>
       <c r="P29" s="42"/>
     </row>
-    <row r="30" spans="1:16" ht="15.75">
+    <row r="30" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="36" t="str">
         <f t="shared" si="0"/>
         <v>terça-feira</v>
@@ -2011,7 +2005,7 @@
       <c r="O30" s="41"/>
       <c r="P30" s="42"/>
     </row>
-    <row r="31" spans="1:16" ht="15.75">
+    <row r="31" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="36" t="str">
         <f t="shared" si="0"/>
         <v>quarta-feira</v>
@@ -2035,7 +2029,7 @@
       <c r="O31" s="41"/>
       <c r="P31" s="42"/>
     </row>
-    <row r="32" spans="1:16" ht="15.75">
+    <row r="32" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="47" t="str">
         <f t="shared" si="0"/>
         <v>quinta-feira</v>
@@ -2059,7 +2053,7 @@
       <c r="O32" s="52"/>
       <c r="P32" s="53"/>
     </row>
-    <row r="33" spans="1:16" ht="15.75">
+    <row r="33" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="47" t="str">
         <f t="shared" si="0"/>
         <v>sexta-feira</v>
@@ -2083,7 +2077,7 @@
       <c r="O33" s="52"/>
       <c r="P33" s="53"/>
     </row>
-    <row r="34" spans="1:16" ht="15.75">
+    <row r="34" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="36" t="str">
         <f t="shared" si="0"/>
         <v>sábado</v>
@@ -2107,7 +2101,7 @@
       <c r="O34" s="41"/>
       <c r="P34" s="42"/>
     </row>
-    <row r="35" spans="1:16" ht="15.75">
+    <row r="35" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="36" t="str">
         <f t="shared" si="0"/>
         <v>domingo</v>
@@ -2131,7 +2125,7 @@
       <c r="O35" s="41"/>
       <c r="P35" s="42"/>
     </row>
-    <row r="36" spans="1:16" ht="15.75">
+    <row r="36" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="36" t="str">
         <f t="shared" si="0"/>
         <v>segunda-feira</v>
@@ -2155,7 +2149,7 @@
       <c r="O36" s="41"/>
       <c r="P36" s="42"/>
     </row>
-    <row r="37" spans="1:16" ht="15.75">
+    <row r="37" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="36" t="str">
         <f t="shared" si="0"/>
         <v>terça-feira</v>
@@ -2179,7 +2173,7 @@
       <c r="O37" s="41"/>
       <c r="P37" s="42"/>
     </row>
-    <row r="38" spans="1:16" ht="15.75">
+    <row r="38" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="36" t="str">
         <f t="shared" si="0"/>
         <v>quarta-feira</v>
@@ -2203,7 +2197,7 @@
       <c r="O38" s="41"/>
       <c r="P38" s="42"/>
     </row>
-    <row r="39" spans="1:16" ht="15.75">
+    <row r="39" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="47" t="str">
         <f>IF(WEEKDAY(B39)=1,"domingo",IF(WEEKDAY(B39)=2,"segunda-feira",IF(WEEKDAY(B39)=3,"terça-feira",IF(WEEKDAY(B39)=4,"quarta-feira",IF(WEEKDAY(B39)=5,"quinta-feira",IF(WEEKDAY(B39)=6,"sexta-feira",IF(WEEKDAY(B39)=7,"sábado","")))))))</f>
         <v>quinta-feira</v>
@@ -2227,7 +2221,7 @@
       <c r="O39" s="52"/>
       <c r="P39" s="53"/>
     </row>
-    <row r="40" spans="1:16" ht="15.75">
+    <row r="40" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="47" t="str">
         <f>IF(WEEKDAY(B40)=1,"domingo",IF(WEEKDAY(B40)=2,"segunda-feira",IF(WEEKDAY(B40)=3,"terça-feira",IF(WEEKDAY(B40)=4,"quarta-feira",IF(WEEKDAY(B40)=5,"quinta-feira",IF(WEEKDAY(B40)=6,"sexta-feira",IF(WEEKDAY(B40)=7,"sábado","")))))))</f>
         <v>sexta-feira</v>
@@ -2251,7 +2245,7 @@
       <c r="O40" s="52"/>
       <c r="P40" s="53"/>
     </row>
-    <row r="41" spans="1:16" ht="15.75">
+    <row r="41" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="36" t="str">
         <f>IF(WEEKDAY(B41)=1,"domingo",IF(WEEKDAY(B41)=2,"segunda-feira",IF(WEEKDAY(B41)=3,"terça-feira",IF(WEEKDAY(B41)=4,"quarta-feira",IF(WEEKDAY(B41)=5,"quinta-feira",IF(WEEKDAY(B41)=6,"sexta-feira",IF(WEEKDAY(B41)=7,"sábado","")))))))</f>
         <v>sábado</v>
@@ -2275,7 +2269,7 @@
       <c r="O41" s="41"/>
       <c r="P41" s="42"/>
     </row>
-    <row r="42" spans="1:16" ht="16.5" thickBot="1">
+    <row r="42" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="36"/>
       <c r="B42" s="37"/>
       <c r="C42" s="38"/>
@@ -2299,15 +2293,15 @@
         <v>0</v>
       </c>
       <c r="N42" s="41" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="O42" s="41"/>
       <c r="P42" s="42"/>
     </row>
-    <row r="43" spans="1:16">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="67"/>
       <c r="B43" s="68" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C43" s="69"/>
       <c r="D43" s="69"/>
@@ -2333,7 +2327,7 @@
       <c r="O43" s="76"/>
       <c r="P43" s="9"/>
     </row>
-    <row r="44" spans="1:16" ht="13.5" thickBot="1">
+    <row r="44" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="67"/>
       <c r="B44" s="70"/>
       <c r="C44" s="71"/>
@@ -2351,7 +2345,7 @@
       <c r="O44" s="77"/>
       <c r="P44" s="10"/>
     </row>
-    <row r="49" spans="7:7">
+    <row r="49" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G49" s="24"/>
     </row>
   </sheetData>

</xml_diff>